<commit_message>
update time data type, from a Time class to a single int
</commit_message>
<xml_diff>
--- a/OutputExcel.xlsx
+++ b/OutputExcel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -29,31 +29,19 @@
     <t>Charger ID</t>
   </si>
   <si>
-    <t>8:0</t>
-  </si>
-  <si>
-    <t>10:20</t>
-  </si>
-  <si>
-    <t>12:0</t>
-  </si>
-  <si>
-    <t>15:56</t>
-  </si>
-  <si>
-    <t>7:0</t>
-  </si>
-  <si>
-    <t>7:24</t>
-  </si>
-  <si>
-    <t>9:0</t>
+    <t>9:00</t>
+  </si>
+  <si>
+    <t>13:42</t>
   </si>
   <si>
     <t>9:27</t>
   </si>
   <si>
-    <t>9:57</t>
+    <t>9:51</t>
+  </si>
+  <si>
+    <t>10:21</t>
   </si>
   <si>
     <t>9:30</t>
@@ -62,13 +50,13 @@
     <t>10:19</t>
   </si>
   <si>
-    <t>11:29</t>
-  </si>
-  <si>
-    <t>11:51</t>
-  </si>
-  <si>
-    <t>12:27</t>
+    <t>11:30</t>
+  </si>
+  <si>
+    <t>11:52</t>
+  </si>
+  <si>
+    <t>12:28</t>
   </si>
   <si>
     <t>12:30</t>
@@ -77,16 +65,22 @@
     <t>13:26</t>
   </si>
   <si>
-    <t>14:1</t>
-  </si>
-  <si>
-    <t>14:49</t>
-  </si>
-  <si>
-    <t>16:25</t>
-  </si>
-  <si>
-    <t>17:13</t>
+    <t>14:01</t>
+  </si>
+  <si>
+    <t>15:14</t>
+  </si>
+  <si>
+    <t>16:50</t>
+  </si>
+  <si>
+    <t>17:33</t>
+  </si>
+  <si>
+    <t>18:20</t>
+  </si>
+  <si>
+    <t>19:08</t>
   </si>
 </sst>
 </file>
@@ -131,7 +125,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -156,10 +150,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>17.0</v>
+        <v>9.0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -173,19 +167,19 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="n">
         <v>2.0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -196,10 +190,10 @@
         <v>3.0</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
         <v>2.0</v>
@@ -207,16 +201,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="B5" t="n">
         <v>3.0</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
         <v>2.0</v>
@@ -224,33 +218,33 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>15.0</v>
+        <v>21.0</v>
       </c>
       <c r="B6" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>21.0</v>
+        <v>18.0</v>
       </c>
       <c r="B7" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
         <v>3.0</v>
@@ -258,16 +252,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="B8" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E8" t="n">
         <v>3.0</v>
@@ -275,16 +269,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4.0</v>
+        <v>27.0</v>
       </c>
       <c r="B9" t="n">
         <v>3.0</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E9" t="n">
         <v>3.0</v>
@@ -292,16 +286,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="B10" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" t="n">
         <v>3.0</v>
@@ -309,16 +303,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>28.0</v>
+        <v>25.0</v>
       </c>
       <c r="B11" t="n">
         <v>1.0</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E11" t="n">
         <v>3.0</v>
@@ -326,16 +320,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>25.0</v>
+        <v>2.0</v>
       </c>
       <c r="B12" t="n">
         <v>1.0</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E12" t="n">
         <v>3.0</v>
@@ -343,16 +337,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>20.0</v>
+        <v>19.0</v>
       </c>
       <c r="B13" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E13" t="n">
         <v>3.0</v>
@@ -360,16 +354,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>19.0</v>
+        <v>7.0</v>
       </c>
       <c r="B14" t="n">
         <v>1.0</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E14" t="n">
         <v>3.0</v>
@@ -377,18 +371,35 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
         <v>16.0</v>
       </c>
-      <c r="B15" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" t="n">
+      <c r="B16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="n">
         <v>3.0</v>
       </c>
     </row>

</xml_diff>